<commit_message>
new channels and fatigue calcs
</commit_message>
<xml_diff>
--- a/bin/material_properties.xlsx
+++ b/bin/material_properties.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexr\OneDrive\Desktop\PSP\Liquids\Propulsion\holistic-engine-logic-program\bin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexr\OneDrive\Desktop\PSP\Liquids\Lander\Propulsion\bin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9109753A-503D-42C4-950B-991284892A6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23437D40-3265-4E42-85CF-2D330790152C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{34498A9F-2ECF-4F9C-8A04-22EC23868BD6}"/>
   </bookViews>
@@ -41,9 +41,6 @@
     <t>Temp (K)</t>
   </si>
   <si>
-    <t>Yeild Strength (MPa)</t>
-  </si>
-  <si>
     <t>CTE (ppm)</t>
   </si>
   <si>
@@ -63,6 +60,9 @@
   </si>
   <si>
     <t>NASA</t>
+  </si>
+  <si>
+    <t>Yield Strength (MPa)</t>
   </si>
 </sst>
 </file>
@@ -161,22 +161,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -494,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA066AC5-B53F-4C28-BBC3-0059A439BC1A}">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -511,36 +508,36 @@
     <col min="11" max="12" width="11.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="29.65" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="29.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>116.14999999999998</v>
       </c>
@@ -561,16 +558,16 @@
         <f>D2/E2</f>
         <v>2793.3333333333335</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="7">
+      <c r="H2" s="5"/>
+      <c r="I2">
         <v>77.594444444444434</v>
       </c>
-      <c r="J2" s="7">
-        <v>79461934113.818359</v>
-      </c>
-      <c r="K2" s="11"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="J2">
+        <v>79461934113.818405</v>
+      </c>
+      <c r="K2" s="8"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>173.14999999999998</v>
       </c>
@@ -591,17 +588,16 @@
         <f t="shared" ref="F3:F9" si="0">D3/E3</f>
         <v>3000</v>
       </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="7">
+      <c r="H3" s="5"/>
+      <c r="I3">
         <v>294.26111111111106</v>
       </c>
-      <c r="J3" s="7">
+      <c r="J3">
         <v>71877714805.774963</v>
       </c>
-      <c r="K3" s="11"/>
-      <c r="L3" s="10"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="K3" s="8"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>223.14999999999998</v>
       </c>
@@ -622,17 +618,16 @@
         <f t="shared" si="0"/>
         <v>2801.5267175572517</v>
       </c>
-      <c r="H4" s="6"/>
-      <c r="I4" s="7">
+      <c r="H4" s="5"/>
+      <c r="I4">
         <v>373.15</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4">
         <v>71188240323.225555</v>
       </c>
-      <c r="K4" s="11"/>
-      <c r="L4" s="10"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="K4" s="8"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>296.14999999999998</v>
       </c>
@@ -653,17 +648,16 @@
         <f t="shared" si="0"/>
         <v>2620.1550387596899</v>
       </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="7">
+      <c r="H5" s="5"/>
+      <c r="I5">
         <v>473.15</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J5">
         <v>58950068257.973709</v>
       </c>
-      <c r="K5" s="11"/>
-      <c r="L5" s="10"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="K5" s="8"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>373.15</v>
       </c>
@@ -684,17 +678,16 @@
         <f t="shared" si="0"/>
         <v>2282.7586206896553</v>
       </c>
-      <c r="H6" s="6"/>
-      <c r="I6" s="7">
+      <c r="H6" s="5"/>
+      <c r="I6">
         <v>573.15</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6">
         <v>37748727919.579651</v>
       </c>
-      <c r="K6" s="11"/>
-      <c r="L6" s="10"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="K6" s="8"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>423.15</v>
       </c>
@@ -711,17 +704,16 @@
         <f t="shared" si="0"/>
         <v>1559.7826086956522</v>
       </c>
-      <c r="H7" s="8"/>
-      <c r="I7" s="9">
+      <c r="H7" s="6"/>
+      <c r="I7" s="7">
         <v>673.15</v>
       </c>
-      <c r="J7" s="9">
+      <c r="J7" s="7">
         <v>19535110338.89967</v>
       </c>
-      <c r="K7" s="11"/>
-      <c r="L7" s="10"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="K7" s="8"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>473.15</v>
       </c>
@@ -739,7 +731,7 @@
         <v>977.27272727272725</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>523.15</v>
       </c>
@@ -757,15 +749,15 @@
         <v>435.81081081081084</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>298.14999999999998</v>
       </c>
@@ -773,7 +765,7 @@
         <v>187.5</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>313.14999999999998</v>
       </c>
@@ -781,7 +773,7 @@
         <v>204.3</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>333.15</v>
       </c>
@@ -789,7 +781,7 @@
         <v>203.5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>353.15</v>
       </c>
@@ -797,7 +789,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>373.15</v>
       </c>
@@ -805,7 +797,7 @@
         <v>207.7</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>393.15</v>
       </c>
@@ -813,7 +805,7 @@
         <v>205.6</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>413.15</v>
       </c>
@@ -821,7 +813,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>433.15</v>
       </c>
@@ -829,28 +821,13 @@
         <v>216.9</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>453.15</v>
       </c>
       <c r="B22">
         <v>218.4</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C28" s="2"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C29" s="2"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C30" s="2"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C31" s="2"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="C32" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>